<commit_message>
Test CSV and text misssing values func
</commit_message>
<xml_diff>
--- a/CLI_Data_Cleaning_Tool/test_excel.xlsx
+++ b/CLI_Data_Cleaning_Tool/test_excel.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Desktop\Python-Backend\Text_Based_Data_Cleaning_Assistant\CLI_Data_Cleaning_Tool\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AFDF96C6-3DD8-464C-9B2A-48DA9DC298AE}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FFEE5C5A-2E72-468A-BD62-902E74CD5BE4}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="16410" windowHeight="7200" xr2:uid="{EB516520-6E83-4BB4-82E1-AE4C4938441F}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="10">
   <si>
     <t>Name</t>
   </si>
@@ -55,9 +55,6 @@
   </si>
   <si>
     <t>Nick</t>
-  </si>
-  <si>
-    <t xml:space="preserve">      nodhiambo01</t>
   </si>
 </sst>
 </file>
@@ -557,9 +554,6 @@
       <c r="A16" t="s">
         <v>9</v>
       </c>
-      <c r="B16" t="s">
-        <v>10</v>
-      </c>
     </row>
   </sheetData>
   <hyperlinks>

</xml_diff>